<commit_message>
CCRU - Template update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - FT NS - CAP.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - FT NS - CAP.xlsx
@@ -12,6 +12,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Traditional Trade'!$A$1:$AL$61</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Traditional Trade'!$A$1:$AL$61</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="275">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -227,15 +228,18 @@
 14</t>
   </si>
   <si>
+    <t xml:space="preserve">Coca-Cola - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of facings</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coca-Cola - 1L</t>
   </si>
   <si>
-    <t xml:space="preserve">Кока-Кола - 1л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of facings</t>
-  </si>
-  <si>
     <t xml:space="preserve">5449000054227, 5449000228970</t>
   </si>
   <si>
@@ -272,19 +276,25 @@
     <t xml:space="preserve">5449000008046</t>
   </si>
   <si>
+    <t xml:space="preserve">Fanta Orange - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Апельсин - 1л</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fanta Orange - 1L</t>
   </si>
   <si>
-    <t xml:space="preserve">Фанта Апельсин - 1л</t>
-  </si>
-  <si>
     <t xml:space="preserve">5449000006271, 5449000228963</t>
   </si>
   <si>
+    <t xml:space="preserve">Sprite - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 1л</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sprite - 1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Спрайт - 1л</t>
   </si>
   <si>
     <t xml:space="preserve">5449000050939, 5449000228956</t>
@@ -980,7 +990,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -989,38 +999,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFCCFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1067,13 +1047,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1140,6 +1120,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1152,14 +1136,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="3" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1168,60 +1144,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="7" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="171" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1237,66 +1169,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF92D050"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF00B050"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -1312,54 +1184,54 @@
   <dimension ref="A1:AMF61"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="22.45"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0404858299595"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8825910931174"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.502024291498"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.8056680161943"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="62.5506072874494"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="40.0283400809717"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7692307692308"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9311740890688"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.4048582995951"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.6882591093117"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.6356275303644"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.919028340081"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.1497975708502"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.1336032388664"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.0890688259109"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.94736842105263"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.8744939271255"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.8663967611336"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="21.4372469635628"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.9676113360324"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="44.5910931174089"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="22.2226720647773"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="24.2712550607287"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="29" min="28" style="0" width="15.1376518218623"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="12.9311740890688"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="12.1457489878543"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="12.6194331983806"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="20.9676113360324"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="77.9838056680162"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="7.5748987854251"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="10.5708502024292"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="9.1497975708502"/>
-    <col collapsed="false" hidden="false" max="1025" min="39" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.9392712550607"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.1417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.8097165991903"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="44.8056680161943"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="64.0283400809717"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="41.0121457489879"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.0404858299595"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.0971659919028"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="26.3238866396761"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="27.2995951417004"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.3441295546559"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="18.4898785425101"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.3481781376518"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="7.09716599190283"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="14.2024291497976"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.2591093117409"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="21.914979757085"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="21.4251012145749"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="45.6599190283401"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="22.7651821862348"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="25.336032388664"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="13.0971659919028"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="12.3603238866397"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="21.4251012145749"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="79.9392712550607"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="7.71255060728745"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="10.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1949,7 +1821,7 @@
       <c r="F9" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="19" t="s">
         <v>61</v>
       </c>
       <c r="H9" s="7" t="s">
@@ -1961,38 +1833,38 @@
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
-      <c r="M9" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="N9" s="20" t="s">
+      <c r="M9" s="20" t="s">
         <v>63</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>64</v>
       </c>
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R9" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
       <c r="V9" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W9" s="7"/>
       <c r="X9" s="7"/>
       <c r="Y9" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z9" s="7"/>
       <c r="AA9" s="7"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD9" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD9" s="10" t="n">
         <v>0.021437</v>
       </c>
       <c r="AE9" s="7"/>
@@ -2029,11 +1901,11 @@
       <c r="E10" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" s="18" t="s">
+      <c r="F10" s="19" t="s">
         <v>70</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>71</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>62</v>
@@ -2044,38 +1916,38 @@
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="N10" s="18" t="s">
-        <v>71</v>
+      <c r="M10" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>72</v>
       </c>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
       <c r="V10" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W10" s="7"/>
       <c r="X10" s="7"/>
       <c r="Y10" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z10" s="7"/>
       <c r="AA10" s="7"/>
       <c r="AB10" s="7"/>
       <c r="AC10" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD10" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD10" s="10" t="n">
         <v>0.021371</v>
       </c>
       <c r="AE10" s="7"/>
@@ -2112,11 +1984,11 @@
       <c r="E11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="18" t="s">
+      <c r="F11" s="19" t="s">
         <v>73</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>74</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>62</v>
@@ -2127,38 +1999,38 @@
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
-      <c r="M11" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="N11" s="18" t="s">
-        <v>74</v>
+      <c r="M11" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
       <c r="V11" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
       <c r="Y11" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD11" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD11" s="10" t="n">
         <v>0.021371</v>
       </c>
       <c r="AE11" s="7"/>
@@ -2196,10 +2068,10 @@
         <v>55</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="G12" s="18" t="s">
         <v>76</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>77</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>62</v>
@@ -2210,38 +2082,38 @@
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
-      <c r="M12" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="N12" s="22" t="s">
-        <v>77</v>
+      <c r="M12" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>79</v>
       </c>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R12" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
       <c r="V12" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W12" s="7"/>
       <c r="X12" s="7"/>
       <c r="Y12" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z12" s="7"/>
       <c r="AA12" s="7"/>
       <c r="AB12" s="7"/>
       <c r="AC12" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD12" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD12" s="10" t="n">
         <v>0.021371</v>
       </c>
       <c r="AE12" s="7"/>
@@ -2279,10 +2151,10 @@
         <v>55</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>62</v>
@@ -2293,38 +2165,38 @@
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="N13" s="20" t="s">
-        <v>80</v>
+      <c r="M13" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>83</v>
       </c>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R13" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
       <c r="V13" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W13" s="7"/>
       <c r="X13" s="7"/>
       <c r="Y13" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z13" s="7"/>
       <c r="AA13" s="7"/>
       <c r="AB13" s="7"/>
       <c r="AC13" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD13" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD13" s="10" t="n">
         <v>0.021371</v>
       </c>
       <c r="AE13" s="7"/>
@@ -2361,11 +2233,11 @@
       <c r="E14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>82</v>
+      <c r="F14" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>62</v>
@@ -2376,38 +2248,38 @@
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
-      <c r="M14" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="N14" s="18" t="s">
-        <v>83</v>
+      <c r="M14" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R14" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
       <c r="V14" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W14" s="7"/>
       <c r="X14" s="7"/>
       <c r="Y14" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z14" s="7"/>
       <c r="AA14" s="7"/>
       <c r="AB14" s="7"/>
       <c r="AC14" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD14" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD14" s="10" t="n">
         <v>0.021371</v>
       </c>
       <c r="AE14" s="7"/>
@@ -2444,11 +2316,11 @@
       <c r="E15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>85</v>
+      <c r="F15" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>62</v>
@@ -2459,38 +2331,38 @@
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
-      <c r="M15" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="N15" s="18" t="s">
-        <v>86</v>
+      <c r="M15" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>89</v>
       </c>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R15" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
       <c r="U15" s="7"/>
       <c r="V15" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
       <c r="Y15" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z15" s="7"/>
       <c r="AA15" s="7"/>
       <c r="AB15" s="7"/>
       <c r="AC15" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD15" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD15" s="10" t="n">
         <v>0.021371</v>
       </c>
       <c r="AE15" s="7"/>
@@ -2527,11 +2399,11 @@
       <c r="E16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>88</v>
+      <c r="F16" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>91</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>62</v>
@@ -2540,38 +2412,38 @@
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
-      <c r="M16" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="N16" s="18" t="s">
-        <v>89</v>
+      <c r="M16" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>92</v>
       </c>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R16" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
       <c r="V16" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="W16" s="7"/>
       <c r="X16" s="7"/>
       <c r="Y16" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z16" s="7"/>
       <c r="AA16" s="7"/>
       <c r="AB16" s="7"/>
       <c r="AC16" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD16" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD16" s="10" t="n">
         <v>0.021371</v>
       </c>
       <c r="AE16" s="7"/>
@@ -2608,11 +2480,11 @@
       <c r="E17" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>92</v>
+      <c r="F17" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>62</v>
@@ -2623,38 +2495,38 @@
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
-      <c r="M17" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="N17" s="18" t="s">
-        <v>93</v>
+      <c r="M17" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="N17" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R17" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
       <c r="V17" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="W17" s="7"/>
       <c r="X17" s="7"/>
       <c r="Y17" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z17" s="7"/>
       <c r="AA17" s="7"/>
       <c r="AB17" s="7"/>
       <c r="AC17" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD17" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD17" s="10" t="n">
         <v>0.010011</v>
       </c>
       <c r="AE17" s="7"/>
@@ -2691,11 +2563,11 @@
       <c r="E18" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>95</v>
+      <c r="F18" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>98</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>62</v>
@@ -2706,38 +2578,38 @@
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
-      <c r="M18" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="N18" s="18" t="s">
-        <v>96</v>
+      <c r="M18" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>99</v>
       </c>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
       <c r="Q18" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R18" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S18" s="7"/>
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
       <c r="V18" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="W18" s="7"/>
       <c r="X18" s="7"/>
       <c r="Y18" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z18" s="7"/>
       <c r="AA18" s="7"/>
       <c r="AB18" s="7"/>
       <c r="AC18" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD18" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD18" s="10" t="n">
         <v>0.009989</v>
       </c>
       <c r="AE18" s="7"/>
@@ -2774,11 +2646,11 @@
       <c r="E19" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>98</v>
+      <c r="F19" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>62</v>
@@ -2789,38 +2661,38 @@
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
-      <c r="M19" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="N19" s="18" t="s">
-        <v>99</v>
+      <c r="M19" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="N19" s="19" t="s">
+        <v>102</v>
       </c>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
       <c r="Q19" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R19" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
       <c r="V19" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
       <c r="Y19" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z19" s="7"/>
       <c r="AA19" s="7"/>
       <c r="AB19" s="7"/>
       <c r="AC19" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD19" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD19" s="10" t="n">
         <v>0.009989</v>
       </c>
       <c r="AE19" s="7"/>
@@ -2857,11 +2729,11 @@
       <c r="E20" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>101</v>
+      <c r="F20" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>62</v>
@@ -2872,38 +2744,38 @@
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
-      <c r="M20" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="N20" s="18" t="s">
-        <v>102</v>
+      <c r="M20" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="N20" s="19" t="s">
+        <v>105</v>
       </c>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
       <c r="V20" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W20" s="7"/>
       <c r="X20" s="7"/>
       <c r="Y20" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z20" s="7"/>
       <c r="AA20" s="7"/>
       <c r="AB20" s="7"/>
       <c r="AC20" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD20" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD20" s="10" t="n">
         <v>0.009989</v>
       </c>
       <c r="AE20" s="7"/>
@@ -2940,11 +2812,11 @@
       <c r="E21" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>104</v>
+      <c r="F21" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>107</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>62</v>
@@ -2955,38 +2827,38 @@
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
-      <c r="M21" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="N21" s="18" t="s">
-        <v>105</v>
+      <c r="M21" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="N21" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
       <c r="Q21" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
       <c r="V21" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W21" s="7"/>
       <c r="X21" s="7"/>
       <c r="Y21" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z21" s="7"/>
       <c r="AA21" s="7"/>
       <c r="AB21" s="7"/>
       <c r="AC21" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD21" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD21" s="10" t="n">
         <v>0.009989</v>
       </c>
       <c r="AE21" s="7"/>
@@ -3021,13 +2893,13 @@
         <v>40</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>58</v>
@@ -3090,13 +2962,13 @@
         <v>40</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F23" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="G23" s="19" t="s">
-        <v>110</v>
+      <c r="F23" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>62</v>
@@ -3107,38 +2979,38 @@
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
-      <c r="M23" s="19" t="s">
-        <v>109</v>
+      <c r="M23" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
       <c r="Q23" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S23" s="7"/>
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
       <c r="V23" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W23" s="7"/>
       <c r="X23" s="7"/>
       <c r="Y23" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z23" s="7"/>
       <c r="AA23" s="7"/>
       <c r="AB23" s="7"/>
       <c r="AC23" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD23" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD23" s="10" t="n">
         <v>0.020999</v>
       </c>
       <c r="AE23" s="7"/>
@@ -3173,13 +3045,13 @@
         <v>40</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>58</v>
@@ -3219,7 +3091,7 @@
         <v>17</v>
       </c>
       <c r="AK24" s="17" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AL24" s="7" t="n">
         <v>300</v>
@@ -3242,13 +3114,13 @@
         <v>40</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>116</v>
+        <v>109</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>119</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>62</v>
@@ -3259,38 +3131,38 @@
       </c>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
-      <c r="M25" s="19" t="s">
-        <v>115</v>
+      <c r="M25" s="20" t="s">
+        <v>118</v>
       </c>
       <c r="N25" s="12" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
       <c r="Q25" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R25" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S25" s="7"/>
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
       <c r="V25" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W25" s="7"/>
       <c r="X25" s="7"/>
       <c r="Y25" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z25" s="7"/>
       <c r="AA25" s="7"/>
       <c r="AB25" s="7"/>
       <c r="AC25" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD25" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD25" s="10" t="n">
         <v>0.020999</v>
       </c>
       <c r="AE25" s="7"/>
@@ -3325,13 +3197,13 @@
         <v>40</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>119</v>
+        <v>109</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>122</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>62</v>
@@ -3342,38 +3214,38 @@
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
-      <c r="M26" s="19" t="s">
-        <v>118</v>
+      <c r="M26" s="20" t="s">
+        <v>121</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
       <c r="Q26" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R26" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S26" s="7"/>
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
       <c r="V26" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
       <c r="Y26" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z26" s="7"/>
       <c r="AA26" s="7"/>
       <c r="AB26" s="7"/>
       <c r="AC26" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD26" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD26" s="10" t="n">
         <v>0.020999</v>
       </c>
       <c r="AE26" s="7"/>
@@ -3408,13 +3280,13 @@
         <v>40</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>58</v>
@@ -3430,7 +3302,7 @@
       <c r="Q27" s="7"/>
       <c r="R27" s="7"/>
       <c r="S27" s="7"/>
-      <c r="T27" s="18"/>
+      <c r="T27" s="19"/>
       <c r="U27" s="7"/>
       <c r="V27" s="7"/>
       <c r="W27" s="7"/>
@@ -3454,7 +3326,7 @@
         <v>20</v>
       </c>
       <c r="AK27" s="17" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AL27" s="7" t="n">
         <v>300</v>
@@ -3477,13 +3349,13 @@
         <v>40</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>62</v>
@@ -3494,38 +3366,38 @@
       </c>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
-      <c r="M28" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="N28" s="23" t="s">
-        <v>127</v>
+      <c r="M28" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="N28" s="22" t="s">
+        <v>130</v>
       </c>
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
       <c r="Q28" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R28" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S28" s="7"/>
       <c r="T28" s="7"/>
       <c r="U28" s="7"/>
       <c r="V28" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W28" s="7"/>
       <c r="X28" s="7"/>
       <c r="Y28" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z28" s="7"/>
       <c r="AA28" s="7"/>
       <c r="AB28" s="7"/>
       <c r="AC28" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD28" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD28" s="10" t="n">
         <v>0.020999</v>
       </c>
       <c r="AE28" s="7"/>
@@ -3560,13 +3432,13 @@
         <v>40</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>62</v>
@@ -3577,38 +3449,38 @@
       </c>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
-      <c r="M29" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="N29" s="23" t="s">
-        <v>130</v>
+      <c r="M29" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="N29" s="22" t="s">
+        <v>133</v>
       </c>
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
       <c r="Q29" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R29" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S29" s="7"/>
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
       <c r="V29" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W29" s="7"/>
       <c r="X29" s="7"/>
       <c r="Y29" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z29" s="7"/>
       <c r="AA29" s="7"/>
       <c r="AB29" s="7"/>
       <c r="AC29" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD29" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD29" s="10" t="n">
         <v>0.010007</v>
       </c>
       <c r="AE29" s="7"/>
@@ -3643,13 +3515,13 @@
         <v>40</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>58</v>
@@ -3689,7 +3561,7 @@
         <v>23</v>
       </c>
       <c r="AK30" s="17" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="AL30" s="7" t="n">
         <v>300</v>
@@ -3712,13 +3584,13 @@
         <v>40</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>135</v>
+        <v>137</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>138</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>62</v>
@@ -3729,38 +3601,38 @@
       </c>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
-      <c r="M31" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="N31" s="18" t="s">
-        <v>136</v>
+      <c r="M31" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="N31" s="19" t="s">
+        <v>139</v>
       </c>
       <c r="O31" s="7"/>
       <c r="P31" s="7"/>
       <c r="Q31" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R31" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S31" s="7"/>
       <c r="T31" s="7"/>
       <c r="U31" s="7"/>
       <c r="V31" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W31" s="7"/>
       <c r="X31" s="7"/>
       <c r="Y31" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z31" s="7"/>
       <c r="AA31" s="7"/>
       <c r="AB31" s="7"/>
       <c r="AC31" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD31" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD31" s="10" t="n">
         <v>0.020999</v>
       </c>
       <c r="AE31" s="7"/>
@@ -3795,13 +3667,13 @@
         <v>40</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>138</v>
+        <v>140</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>141</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>62</v>
@@ -3812,38 +3684,38 @@
       </c>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
-      <c r="M32" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="N32" s="18" t="s">
-        <v>139</v>
+      <c r="M32" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="N32" s="19" t="s">
+        <v>142</v>
       </c>
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
       <c r="Q32" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R32" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S32" s="7"/>
       <c r="T32" s="7"/>
       <c r="U32" s="7"/>
       <c r="V32" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W32" s="7"/>
       <c r="X32" s="7"/>
       <c r="Y32" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z32" s="7"/>
       <c r="AA32" s="7"/>
       <c r="AB32" s="7"/>
       <c r="AC32" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD32" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD32" s="10" t="n">
         <v>0.020999</v>
       </c>
       <c r="AE32" s="7"/>
@@ -3878,13 +3750,13 @@
         <v>40</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>141</v>
+        <v>143</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>144</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>62</v>
@@ -3895,38 +3767,38 @@
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
-      <c r="M33" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="N33" s="18" t="s">
-        <v>142</v>
+      <c r="M33" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="N33" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
       <c r="Q33" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R33" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S33" s="7"/>
       <c r="T33" s="7"/>
       <c r="U33" s="7"/>
       <c r="V33" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W33" s="7"/>
       <c r="X33" s="7"/>
       <c r="Y33" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z33" s="7"/>
       <c r="AA33" s="7"/>
       <c r="AB33" s="7"/>
       <c r="AC33" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD33" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD33" s="10" t="n">
         <v>0.020999</v>
       </c>
       <c r="AE33" s="7"/>
@@ -3961,13 +3833,13 @@
         <v>40</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>147</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>62</v>
@@ -3978,38 +3850,38 @@
       </c>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
-      <c r="M34" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="N34" s="18" t="s">
-        <v>145</v>
+      <c r="M34" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="N34" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
       <c r="Q34" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R34" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S34" s="7"/>
       <c r="T34" s="7"/>
       <c r="U34" s="7"/>
       <c r="V34" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W34" s="7"/>
       <c r="X34" s="7"/>
       <c r="Y34" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z34" s="7"/>
       <c r="AA34" s="7"/>
       <c r="AB34" s="7"/>
       <c r="AC34" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD34" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD34" s="10" t="n">
         <v>0.020999</v>
       </c>
       <c r="AE34" s="7"/>
@@ -4044,13 +3916,13 @@
         <v>40</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="G35" s="19" t="s">
-        <v>147</v>
+        <v>149</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>150</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>62</v>
@@ -4061,38 +3933,38 @@
       </c>
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
-      <c r="M35" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="N35" s="18" t="s">
-        <v>148</v>
+      <c r="M35" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="N35" s="19" t="s">
+        <v>151</v>
       </c>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R35" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S35" s="7"/>
       <c r="T35" s="7"/>
       <c r="U35" s="7"/>
       <c r="V35" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W35" s="7"/>
       <c r="X35" s="7"/>
       <c r="Y35" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z35" s="7"/>
       <c r="AA35" s="7"/>
       <c r="AB35" s="7"/>
       <c r="AC35" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD35" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD35" s="10" t="n">
         <v>0.020999</v>
       </c>
       <c r="AE35" s="7"/>
@@ -4127,13 +3999,13 @@
         <v>40</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>150</v>
+        <v>152</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>153</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>62</v>
@@ -4144,38 +4016,38 @@
       </c>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
-      <c r="M36" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="N36" s="18" t="s">
-        <v>151</v>
+      <c r="M36" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="N36" s="19" t="s">
+        <v>154</v>
       </c>
       <c r="O36" s="7"/>
       <c r="P36" s="7"/>
       <c r="Q36" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R36" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S36" s="7"/>
       <c r="T36" s="7"/>
       <c r="U36" s="7"/>
       <c r="V36" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W36" s="7"/>
       <c r="X36" s="7"/>
       <c r="Y36" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z36" s="7"/>
       <c r="AA36" s="7"/>
       <c r="AB36" s="7"/>
       <c r="AC36" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD36" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD36" s="10" t="n">
         <v>0.010007</v>
       </c>
       <c r="AE36" s="7"/>
@@ -4210,13 +4082,13 @@
         <v>40</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>62</v>
@@ -4227,41 +4099,41 @@
       </c>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
-      <c r="M37" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="N37" s="18" t="s">
-        <v>154</v>
+      <c r="M37" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="N37" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="O37" s="12"/>
       <c r="P37" s="12"/>
       <c r="Q37" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R37" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S37" s="7"/>
       <c r="T37" s="7"/>
       <c r="U37" s="7"/>
       <c r="V37" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W37" s="7"/>
       <c r="X37" s="7"/>
       <c r="Y37" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z37" s="7"/>
       <c r="AA37" s="7"/>
       <c r="AB37" s="7"/>
       <c r="AC37" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD37" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD37" s="10" t="n">
         <v>0.010007</v>
       </c>
-      <c r="AE37" s="18"/>
+      <c r="AE37" s="19"/>
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
       <c r="AH37" s="7"/>
@@ -4293,13 +4165,13 @@
         <v>40</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="G38" s="19" t="s">
-        <v>156</v>
+        <v>158</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>159</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>62</v>
@@ -4310,38 +4182,38 @@
       </c>
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
-      <c r="M38" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="N38" s="18" t="s">
-        <v>157</v>
+      <c r="M38" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="N38" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="O38" s="7"/>
       <c r="P38" s="7"/>
       <c r="Q38" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R38" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S38" s="7"/>
       <c r="T38" s="7"/>
       <c r="U38" s="7"/>
       <c r="V38" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W38" s="7"/>
       <c r="X38" s="7"/>
       <c r="Y38" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z38" s="7"/>
       <c r="AA38" s="7"/>
       <c r="AB38" s="7"/>
       <c r="AC38" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD38" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD38" s="10" t="n">
         <v>0.009987</v>
       </c>
       <c r="AE38" s="7"/>
@@ -4376,7 +4248,7 @@
         <v>40</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>45</v>
@@ -4385,7 +4257,7 @@
         <v>46</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="9" t="n">
@@ -4398,15 +4270,15 @@
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
       <c r="Q39" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R39" s="7"/>
       <c r="S39" s="7"/>
       <c r="T39" s="7"/>
-      <c r="U39" s="24"/>
+      <c r="U39" s="23"/>
       <c r="V39" s="7"/>
       <c r="W39" s="7" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="X39" s="7"/>
       <c r="Y39" s="7"/>
@@ -4414,9 +4286,9 @@
       <c r="AA39" s="7"/>
       <c r="AB39" s="7"/>
       <c r="AC39" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD39" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD39" s="10" t="n">
         <v>0.15</v>
       </c>
       <c r="AE39" s="7"/>
@@ -4430,9 +4302,9 @@
         <v>32</v>
       </c>
       <c r="AK39" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="AL39" s="25" t="n">
+        <v>164</v>
+      </c>
+      <c r="AL39" s="19" t="n">
         <v>303</v>
       </c>
       <c r="AMD39" s="6"/>
@@ -4453,13 +4325,13 @@
         <v>40</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>62</v>
@@ -4471,25 +4343,25 @@
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
       <c r="M40" s="7" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="N40" s="12" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="O40" s="12"/>
       <c r="P40" s="12"/>
       <c r="Q40" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R40" s="7" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="S40" s="7"/>
       <c r="T40" s="7"/>
-      <c r="U40" s="24"/>
+      <c r="U40" s="23"/>
       <c r="V40" s="7"/>
       <c r="W40" s="7" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="X40" s="7"/>
       <c r="Y40" s="7"/>
@@ -4497,7 +4369,7 @@
       <c r="AA40" s="7"/>
       <c r="AB40" s="7"/>
       <c r="AC40" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD40" s="10"/>
       <c r="AE40" s="7"/>
@@ -4532,16 +4404,16 @@
         <v>40</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="I41" s="7"/>
       <c r="J41" s="9" t="n">
@@ -4554,15 +4426,15 @@
       <c r="O41" s="12"/>
       <c r="P41" s="12"/>
       <c r="Q41" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R41" s="7"/>
       <c r="S41" s="7"/>
       <c r="T41" s="7"/>
-      <c r="U41" s="24"/>
+      <c r="U41" s="23"/>
       <c r="V41" s="7"/>
       <c r="W41" s="7" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="X41" s="7"/>
       <c r="Y41" s="7"/>
@@ -4570,7 +4442,7 @@
       <c r="AA41" s="7"/>
       <c r="AB41" s="7"/>
       <c r="AC41" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD41" s="10"/>
       <c r="AE41" s="7"/>
@@ -4584,7 +4456,7 @@
         <v>34</v>
       </c>
       <c r="AK41" s="17" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="AL41" s="7" t="n">
         <v>32</v>
@@ -4607,23 +4479,23 @@
         <v>40</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
       <c r="L42" s="9"/>
       <c r="M42" s="7" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="N42" s="12" t="n">
         <v>4607042434877</v>
@@ -4631,17 +4503,17 @@
       <c r="O42" s="12"/>
       <c r="P42" s="12"/>
       <c r="Q42" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R42" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S42" s="7"/>
       <c r="T42" s="7"/>
-      <c r="U42" s="24"/>
+      <c r="U42" s="23"/>
       <c r="V42" s="7"/>
       <c r="W42" s="7" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="X42" s="7"/>
       <c r="Y42" s="7"/>
@@ -4649,14 +4521,14 @@
       <c r="AA42" s="7"/>
       <c r="AB42" s="7"/>
       <c r="AC42" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD42" s="10"/>
       <c r="AE42" s="7"/>
       <c r="AF42" s="7"/>
       <c r="AG42" s="7"/>
       <c r="AH42" s="7" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AI42" s="7" t="n">
         <v>4</v>
@@ -4686,41 +4558,41 @@
         <v>40</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G43" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="H43" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>173</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
       <c r="L43" s="9"/>
       <c r="M43" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="N43" s="18" t="s">
-        <v>139</v>
+        <v>140</v>
+      </c>
+      <c r="N43" s="19" t="s">
+        <v>142</v>
       </c>
       <c r="O43" s="12"/>
       <c r="P43" s="12"/>
       <c r="Q43" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R43" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S43" s="7"/>
       <c r="T43" s="7"/>
-      <c r="U43" s="24"/>
+      <c r="U43" s="23"/>
       <c r="V43" s="7"/>
       <c r="W43" s="7" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="X43" s="7"/>
       <c r="Y43" s="7"/>
@@ -4728,14 +4600,14 @@
       <c r="AA43" s="7"/>
       <c r="AB43" s="7"/>
       <c r="AC43" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD43" s="10"/>
       <c r="AE43" s="7"/>
       <c r="AF43" s="7"/>
       <c r="AG43" s="7"/>
       <c r="AH43" s="7" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="AI43" s="7" t="n">
         <v>4</v>
@@ -4765,19 +4637,19 @@
         <v>40</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="I44" s="7"/>
-      <c r="J44" s="26"/>
+      <c r="J44" s="24"/>
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
       <c r="M44" s="7"/>
@@ -4785,7 +4657,7 @@
       <c r="O44" s="12"/>
       <c r="P44" s="12"/>
       <c r="Q44" s="7" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="R44" s="7"/>
       <c r="S44" s="7"/>
@@ -4799,16 +4671,16 @@
       <c r="AA44" s="7"/>
       <c r="AB44" s="7"/>
       <c r="AC44" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="AD44" s="21" t="n">
+        <v>186</v>
+      </c>
+      <c r="AD44" s="10" t="n">
         <v>0.24</v>
       </c>
       <c r="AE44" s="7"/>
       <c r="AF44" s="7"/>
       <c r="AG44" s="7"/>
       <c r="AH44" s="7" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="AI44" s="7" t="n">
         <v>2</v>
@@ -4817,7 +4689,7 @@
         <v>36</v>
       </c>
       <c r="AK44" s="17" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="AL44" s="16" t="n">
         <v>311</v>
@@ -4840,16 +4712,16 @@
         <v>40</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="I45" s="7"/>
       <c r="J45" s="9" t="n">
@@ -4860,42 +4732,42 @@
       </c>
       <c r="L45" s="9"/>
       <c r="M45" s="7" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="N45" s="12" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O45" s="12"/>
       <c r="P45" s="12"/>
       <c r="Q45" s="7"/>
       <c r="R45" s="7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="S45" s="7"/>
       <c r="T45" s="7"/>
       <c r="U45" s="7"/>
       <c r="V45" s="7"/>
       <c r="W45" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="X45" s="7"/>
       <c r="Y45" s="7" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="Z45" s="7"/>
       <c r="AA45" s="7"/>
       <c r="AB45" s="7"/>
       <c r="AC45" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD45" s="10"/>
       <c r="AE45" s="7"/>
       <c r="AF45" s="7"/>
       <c r="AG45" s="7" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="AH45" s="7" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="AI45" s="7" t="n">
         <v>3</v>
@@ -4925,16 +4797,16 @@
         <v>40</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="I46" s="7"/>
       <c r="J46" s="9" t="n">
@@ -4945,42 +4817,42 @@
       </c>
       <c r="L46" s="9"/>
       <c r="M46" s="7" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="N46" s="12" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O46" s="12"/>
       <c r="P46" s="12"/>
       <c r="Q46" s="7"/>
       <c r="R46" s="7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="S46" s="7"/>
       <c r="T46" s="7"/>
       <c r="U46" s="7"/>
       <c r="V46" s="7"/>
       <c r="W46" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="X46" s="7" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="Y46" s="7"/>
       <c r="Z46" s="7"/>
       <c r="AA46" s="7"/>
       <c r="AB46" s="7"/>
       <c r="AC46" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD46" s="10"/>
       <c r="AE46" s="7"/>
       <c r="AF46" s="7"/>
       <c r="AG46" s="7" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="AH46" s="7" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="AI46" s="7" t="n">
         <v>3</v>
@@ -5010,16 +4882,16 @@
         <v>40</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="9" t="n">
@@ -5028,23 +4900,23 @@
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
       <c r="M47" s="7" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="N47" s="12" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O47" s="12"/>
       <c r="P47" s="12"/>
       <c r="Q47" s="7"/>
       <c r="R47" s="7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="S47" s="7"/>
       <c r="T47" s="7"/>
       <c r="U47" s="7"/>
       <c r="V47" s="7"/>
       <c r="W47" s="7" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="X47" s="7"/>
       <c r="Y47" s="7"/>
@@ -5052,7 +4924,7 @@
       <c r="AA47" s="7"/>
       <c r="AB47" s="7"/>
       <c r="AC47" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD47" s="10"/>
       <c r="AE47" s="7"/>
@@ -5087,18 +4959,18 @@
         <v>40</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="I48" s="18"/>
+        <v>209</v>
+      </c>
+      <c r="I48" s="19"/>
       <c r="J48" s="9" t="n">
         <v>1</v>
       </c>
@@ -5106,41 +4978,41 @@
       <c r="L48" s="9"/>
       <c r="M48" s="7"/>
       <c r="N48" s="7" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="O48" s="12"/>
       <c r="P48" s="12"/>
       <c r="Q48" s="7"/>
       <c r="R48" s="7" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="S48" s="7"/>
       <c r="T48" s="7"/>
       <c r="U48" s="7"/>
       <c r="V48" s="7"/>
       <c r="W48" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="X48" s="7" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="Y48" s="7"/>
       <c r="Z48" s="7"/>
       <c r="AA48" s="7"/>
       <c r="AB48" s="7"/>
       <c r="AC48" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD48" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD48" s="10" t="n">
         <v>0.04</v>
       </c>
       <c r="AE48" s="7"/>
       <c r="AF48" s="7"/>
       <c r="AG48" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AH48" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="AI48" s="7" t="n">
         <v>2</v>
@@ -5149,7 +5021,7 @@
         <v>40</v>
       </c>
       <c r="AK48" s="7"/>
-      <c r="AL48" s="27" t="n">
+      <c r="AL48" s="25" t="n">
         <v>312</v>
       </c>
       <c r="AMD48" s="6"/>
@@ -5170,18 +5042,18 @@
         <v>40</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="H49" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="I49" s="18"/>
+        <v>214</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="I49" s="19"/>
       <c r="J49" s="9"/>
       <c r="K49" s="9" t="n">
         <v>1</v>
@@ -5190,44 +5062,44 @@
         <v>15</v>
       </c>
       <c r="M49" s="7" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="N49" s="12" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O49" s="12"/>
       <c r="P49" s="12"/>
       <c r="Q49" s="7"/>
       <c r="R49" s="7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="S49" s="7"/>
       <c r="T49" s="7"/>
       <c r="U49" s="7"/>
       <c r="V49" s="7"/>
       <c r="W49" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="X49" s="7"/>
       <c r="Y49" s="7" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="Z49" s="7"/>
       <c r="AA49" s="7"/>
       <c r="AB49" s="7"/>
       <c r="AC49" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD49" s="21" t="n">
+        <v>69</v>
+      </c>
+      <c r="AD49" s="10" t="n">
         <v>0.04</v>
       </c>
       <c r="AE49" s="7"/>
       <c r="AF49" s="7"/>
       <c r="AG49" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AH49" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="AI49" s="7" t="n">
         <v>2</v>
@@ -5236,7 +5108,7 @@
         <v>41</v>
       </c>
       <c r="AK49" s="7"/>
-      <c r="AL49" s="27" t="n">
+      <c r="AL49" s="25" t="n">
         <v>312</v>
       </c>
       <c r="AMD49" s="6"/>
@@ -5257,18 +5129,18 @@
         <v>40</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="H50" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I50" s="18"/>
+      <c r="I50" s="19"/>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
       <c r="L50" s="9"/>
@@ -5277,7 +5149,7 @@
       <c r="O50" s="12"/>
       <c r="P50" s="12"/>
       <c r="Q50" s="7" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="R50" s="7"/>
       <c r="S50" s="7"/>
@@ -5285,7 +5157,7 @@
       <c r="U50" s="7"/>
       <c r="V50" s="7"/>
       <c r="W50" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="X50" s="7"/>
       <c r="Y50" s="7"/>
@@ -5293,18 +5165,18 @@
       <c r="AA50" s="7"/>
       <c r="AB50" s="7"/>
       <c r="AC50" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="AD50" s="21" t="n">
+        <v>186</v>
+      </c>
+      <c r="AD50" s="10" t="n">
         <v>0.04</v>
       </c>
       <c r="AE50" s="7"/>
       <c r="AF50" s="7"/>
       <c r="AG50" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AH50" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="AI50" s="7" t="n">
         <v>2</v>
@@ -5313,9 +5185,9 @@
         <v>42</v>
       </c>
       <c r="AK50" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="AL50" s="27" t="n">
+        <v>219</v>
+      </c>
+      <c r="AL50" s="25" t="n">
         <v>312</v>
       </c>
       <c r="AMD50" s="6"/>
@@ -5337,61 +5209,61 @@
       </c>
       <c r="E51" s="7"/>
       <c r="F51" s="7" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="I51" s="18"/>
+        <v>222</v>
+      </c>
+      <c r="I51" s="19"/>
       <c r="J51" s="9" t="n">
         <v>0.4</v>
       </c>
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
       <c r="M51" s="7" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="N51" s="12" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="O51" s="12"/>
       <c r="P51" s="12" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="Q51" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="R51" s="29" t="s">
-        <v>222</v>
+        <v>65</v>
+      </c>
+      <c r="R51" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="S51" s="7"/>
       <c r="T51" s="7"/>
       <c r="U51" s="7"/>
       <c r="V51" s="7"/>
       <c r="W51" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="X51" s="7" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="Y51" s="7"/>
       <c r="Z51" s="7"/>
       <c r="AA51" s="7"/>
       <c r="AB51" s="7"/>
       <c r="AC51" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD51" s="10"/>
       <c r="AE51" s="7"/>
       <c r="AF51" s="7"/>
       <c r="AG51" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AH51" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="AI51" s="7" t="n">
         <v>3</v>
@@ -5419,15 +5291,15 @@
       </c>
       <c r="E52" s="7"/>
       <c r="F52" s="7" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="I52" s="18"/>
+        <v>172</v>
+      </c>
+      <c r="I52" s="19"/>
       <c r="J52" s="9" t="n">
         <v>2</v>
       </c>
@@ -5438,7 +5310,7 @@
       <c r="O52" s="12"/>
       <c r="P52" s="12"/>
       <c r="Q52" s="7" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="R52" s="7"/>
       <c r="S52" s="7"/>
@@ -5446,7 +5318,7 @@
       <c r="U52" s="7"/>
       <c r="V52" s="7"/>
       <c r="W52" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="X52" s="7"/>
       <c r="Y52" s="7"/>
@@ -5454,16 +5326,16 @@
       <c r="AA52" s="7"/>
       <c r="AB52" s="7"/>
       <c r="AC52" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD52" s="10"/>
       <c r="AE52" s="7"/>
       <c r="AF52" s="7"/>
       <c r="AG52" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AH52" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="AI52" s="7" t="n">
         <v>3</v>
@@ -5472,7 +5344,7 @@
         <v>45</v>
       </c>
       <c r="AK52" s="17" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="AL52" s="7" t="n">
         <v>42</v>
@@ -5493,10 +5365,10 @@
       </c>
       <c r="E53" s="7"/>
       <c r="F53" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="G53" s="30" t="s">
-        <v>228</v>
+        <v>230</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>231</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>62</v>
@@ -5506,50 +5378,50 @@
         <v>4</v>
       </c>
       <c r="K53" s="9"/>
-      <c r="L53" s="31"/>
-      <c r="M53" s="30" t="s">
-        <v>229</v>
-      </c>
-      <c r="N53" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="O53" s="32"/>
-      <c r="P53" s="32" t="s">
-        <v>230</v>
+      <c r="L53" s="26"/>
+      <c r="M53" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="N53" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="O53" s="12"/>
+      <c r="P53" s="12" t="s">
+        <v>233</v>
       </c>
       <c r="Q53" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="R53" s="29" t="s">
-        <v>222</v>
+        <v>65</v>
+      </c>
+      <c r="R53" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="S53" s="7"/>
       <c r="T53" s="7"/>
       <c r="U53" s="7"/>
       <c r="V53" s="7"/>
       <c r="W53" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="X53" s="17" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="Y53" s="7"/>
       <c r="Z53" s="7"/>
       <c r="AA53" s="7"/>
       <c r="AB53" s="7" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="AC53" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD53" s="10"/>
       <c r="AE53" s="7"/>
       <c r="AF53" s="7"/>
       <c r="AG53" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AH53" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="AI53" s="7" t="n">
         <v>4</v>
@@ -5577,10 +5449,10 @@
       </c>
       <c r="E54" s="7"/>
       <c r="F54" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="G54" s="30" t="s">
-        <v>234</v>
+        <v>236</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>237</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>62</v>
@@ -5591,49 +5463,49 @@
       </c>
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
-      <c r="M54" s="30" t="s">
-        <v>235</v>
-      </c>
-      <c r="N54" s="32" t="s">
-        <v>221</v>
-      </c>
-      <c r="O54" s="32"/>
-      <c r="P54" s="32" t="s">
-        <v>221</v>
+      <c r="M54" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="N54" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="O54" s="12"/>
+      <c r="P54" s="12" t="s">
+        <v>224</v>
       </c>
       <c r="Q54" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="R54" s="29" t="s">
-        <v>222</v>
+        <v>65</v>
+      </c>
+      <c r="R54" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="S54" s="7"/>
       <c r="T54" s="7"/>
       <c r="U54" s="7"/>
       <c r="V54" s="7"/>
       <c r="W54" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="X54" s="17" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="Y54" s="7"/>
       <c r="Z54" s="7"/>
       <c r="AA54" s="7"/>
       <c r="AB54" s="7" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="AC54" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD54" s="10"/>
       <c r="AE54" s="7"/>
       <c r="AF54" s="7"/>
       <c r="AG54" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AH54" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="AI54" s="7" t="n">
         <v>4</v>
@@ -5661,59 +5533,59 @@
       </c>
       <c r="E55" s="7"/>
       <c r="F55" s="7" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="H55" s="28" t="s">
-        <v>239</v>
-      </c>
-      <c r="I55" s="18"/>
+        <v>241</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="I55" s="19"/>
       <c r="J55" s="9" t="n">
         <v>2</v>
       </c>
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
       <c r="M55" s="7" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="N55" s="12" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O55" s="12"/>
       <c r="P55" s="12"/>
       <c r="Q55" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="R55" s="29" t="s">
-        <v>191</v>
+        <v>65</v>
+      </c>
+      <c r="R55" s="7" t="s">
+        <v>194</v>
       </c>
       <c r="S55" s="7"/>
       <c r="T55" s="7"/>
       <c r="U55" s="7"/>
       <c r="V55" s="7"/>
       <c r="W55" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="X55" s="17" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="Y55" s="7"/>
       <c r="Z55" s="7"/>
       <c r="AA55" s="7"/>
       <c r="AB55" s="7"/>
       <c r="AC55" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD55" s="10"/>
       <c r="AE55" s="7"/>
       <c r="AF55" s="7"/>
       <c r="AG55" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AH55" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="AI55" s="7" t="n">
         <v>3</v>
@@ -5740,16 +5612,16 @@
         <v>40</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="I56" s="7"/>
       <c r="J56" s="9"/>
@@ -5757,20 +5629,20 @@
       <c r="L56" s="9"/>
       <c r="M56" s="7"/>
       <c r="N56" s="12" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="O56" s="12"/>
       <c r="P56" s="12"/>
       <c r="Q56" s="7"/>
       <c r="R56" s="7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="S56" s="7"/>
       <c r="T56" s="7"/>
       <c r="U56" s="7"/>
       <c r="V56" s="7"/>
       <c r="W56" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="X56" s="7"/>
       <c r="Y56" s="7"/>
@@ -5778,18 +5650,18 @@
       <c r="AA56" s="7"/>
       <c r="AB56" s="7"/>
       <c r="AC56" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="AD56" s="21" t="n">
+        <v>186</v>
+      </c>
+      <c r="AD56" s="10" t="n">
         <v>0.04</v>
       </c>
       <c r="AE56" s="7"/>
       <c r="AF56" s="7"/>
       <c r="AG56" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AH56" s="7" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="AI56" s="7" t="n">
         <v>2</v>
@@ -5798,273 +5670,273 @@
         <v>49</v>
       </c>
       <c r="AK56" s="7"/>
-      <c r="AL56" s="27" t="n">
+      <c r="AL56" s="25" t="n">
         <v>312</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="33" t="n">
+      <c r="A57" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="B57" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C57" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D57" s="33" t="s">
-        <v>243</v>
-      </c>
-      <c r="E57" s="34" t="s">
-        <v>244</v>
-      </c>
-      <c r="F57" s="34" t="s">
-        <v>245</v>
-      </c>
-      <c r="G57" s="34" t="s">
+      <c r="B57" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="H57" s="33" t="s">
+      <c r="E57" s="25" t="s">
         <v>247</v>
       </c>
-      <c r="I57" s="33" t="s">
+      <c r="F57" s="25" t="s">
         <v>248</v>
       </c>
-      <c r="J57" s="35"/>
-      <c r="K57" s="35"/>
-      <c r="L57" s="35"/>
-      <c r="M57" s="33"/>
-      <c r="N57" s="33"/>
-      <c r="O57" s="33"/>
-      <c r="P57" s="33"/>
-      <c r="Q57" s="33"/>
-      <c r="R57" s="33" t="s">
+      <c r="G57" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="S57" s="33"/>
-      <c r="T57" s="33"/>
-      <c r="U57" s="33"/>
-      <c r="V57" s="33"/>
-      <c r="W57" s="33"/>
-      <c r="X57" s="33"/>
-      <c r="Y57" s="33"/>
-      <c r="Z57" s="33"/>
-      <c r="AA57" s="33"/>
-      <c r="AB57" s="33"/>
-      <c r="AC57" s="33"/>
-      <c r="AD57" s="36"/>
-      <c r="AE57" s="33"/>
-      <c r="AF57" s="33"/>
-      <c r="AG57" s="33"/>
-      <c r="AH57" s="33"/>
-      <c r="AI57" s="33"/>
-      <c r="AJ57" s="33" t="n">
+      <c r="H57" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="7"/>
+      <c r="P57" s="7"/>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="S57" s="7"/>
+      <c r="T57" s="7"/>
+      <c r="U57" s="7"/>
+      <c r="V57" s="7"/>
+      <c r="W57" s="7"/>
+      <c r="X57" s="7"/>
+      <c r="Y57" s="7"/>
+      <c r="Z57" s="7"/>
+      <c r="AA57" s="7"/>
+      <c r="AB57" s="7"/>
+      <c r="AC57" s="7"/>
+      <c r="AD57" s="10"/>
+      <c r="AE57" s="7"/>
+      <c r="AF57" s="7"/>
+      <c r="AG57" s="7"/>
+      <c r="AH57" s="7"/>
+      <c r="AI57" s="7"/>
+      <c r="AJ57" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="AK57" s="37" t="s">
-        <v>250</v>
-      </c>
-      <c r="AL57" s="33"/>
+      <c r="AK57" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="AL57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="33" t="n">
+      <c r="A58" s="7" t="n">
         <v>51</v>
       </c>
-      <c r="B58" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C58" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D58" s="33" t="s">
-        <v>243</v>
-      </c>
-      <c r="E58" s="34" t="s">
+      <c r="B58" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E58" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="F58" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="G58" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="I58" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="F58" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="G58" s="34" t="s">
-        <v>253</v>
-      </c>
-      <c r="H58" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="I58" s="33" t="s">
-        <v>248</v>
-      </c>
-      <c r="J58" s="35"/>
-      <c r="K58" s="35"/>
-      <c r="L58" s="35"/>
-      <c r="M58" s="33"/>
-      <c r="N58" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="O58" s="33"/>
-      <c r="P58" s="33"/>
-      <c r="Q58" s="33"/>
-      <c r="R58" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="S58" s="33"/>
-      <c r="T58" s="33"/>
-      <c r="U58" s="33"/>
-      <c r="V58" s="33"/>
-      <c r="W58" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="X58" s="37" t="s">
-        <v>257</v>
-      </c>
-      <c r="Y58" s="33"/>
-      <c r="Z58" s="33"/>
-      <c r="AA58" s="33"/>
-      <c r="AB58" s="33"/>
-      <c r="AC58" s="33"/>
-      <c r="AD58" s="36"/>
-      <c r="AE58" s="33"/>
-      <c r="AF58" s="33"/>
-      <c r="AG58" s="33"/>
-      <c r="AH58" s="33"/>
-      <c r="AI58" s="33"/>
-      <c r="AJ58" s="33" t="n">
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="7"/>
+      <c r="N58" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="O58" s="7"/>
+      <c r="P58" s="7"/>
+      <c r="Q58" s="7"/>
+      <c r="R58" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="S58" s="7"/>
+      <c r="T58" s="7"/>
+      <c r="U58" s="7"/>
+      <c r="V58" s="7"/>
+      <c r="W58" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="X58" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y58" s="7"/>
+      <c r="Z58" s="7"/>
+      <c r="AA58" s="7"/>
+      <c r="AB58" s="7"/>
+      <c r="AC58" s="7"/>
+      <c r="AD58" s="10"/>
+      <c r="AE58" s="7"/>
+      <c r="AF58" s="7"/>
+      <c r="AG58" s="7"/>
+      <c r="AH58" s="7"/>
+      <c r="AI58" s="7"/>
+      <c r="AJ58" s="7" t="n">
         <v>51</v>
       </c>
-      <c r="AK58" s="33"/>
-      <c r="AL58" s="33"/>
+      <c r="AK58" s="7"/>
+      <c r="AL58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="33" t="n">
+      <c r="A59" s="7" t="n">
         <v>52</v>
       </c>
-      <c r="B59" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C59" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D59" s="33" t="s">
-        <v>243</v>
-      </c>
-      <c r="E59" s="34" t="s">
-        <v>258</v>
-      </c>
-      <c r="F59" s="34" t="s">
+      <c r="B59" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="F59" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="G59" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="7"/>
+      <c r="N59" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="O59" s="7"/>
+      <c r="P59" s="7"/>
+      <c r="Q59" s="7"/>
+      <c r="R59" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="G59" s="34" t="s">
-        <v>260</v>
-      </c>
-      <c r="H59" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="I59" s="33" t="s">
-        <v>262</v>
-      </c>
-      <c r="J59" s="35"/>
-      <c r="K59" s="35"/>
-      <c r="L59" s="35"/>
-      <c r="M59" s="33"/>
-      <c r="N59" s="33" t="s">
-        <v>263</v>
-      </c>
-      <c r="O59" s="33"/>
-      <c r="P59" s="33"/>
-      <c r="Q59" s="33"/>
-      <c r="R59" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="S59" s="33"/>
-      <c r="T59" s="33"/>
-      <c r="U59" s="33"/>
-      <c r="V59" s="33"/>
-      <c r="W59" s="33"/>
+      <c r="S59" s="7"/>
+      <c r="T59" s="7"/>
+      <c r="U59" s="7"/>
+      <c r="V59" s="7"/>
+      <c r="W59" s="7"/>
       <c r="X59" s="17" t="s">
-        <v>264</v>
-      </c>
-      <c r="Y59" s="33"/>
-      <c r="Z59" s="33"/>
-      <c r="AA59" s="33"/>
-      <c r="AB59" s="33"/>
-      <c r="AC59" s="33"/>
-      <c r="AD59" s="36"/>
-      <c r="AE59" s="33"/>
-      <c r="AF59" s="33"/>
-      <c r="AG59" s="33"/>
-      <c r="AH59" s="33"/>
-      <c r="AI59" s="33"/>
-      <c r="AJ59" s="33" t="n">
+        <v>267</v>
+      </c>
+      <c r="Y59" s="7"/>
+      <c r="Z59" s="7"/>
+      <c r="AA59" s="7"/>
+      <c r="AB59" s="7"/>
+      <c r="AC59" s="7"/>
+      <c r="AD59" s="10"/>
+      <c r="AE59" s="7"/>
+      <c r="AF59" s="7"/>
+      <c r="AG59" s="7"/>
+      <c r="AH59" s="7"/>
+      <c r="AI59" s="7"/>
+      <c r="AJ59" s="7" t="n">
         <v>52</v>
       </c>
-      <c r="AK59" s="33"/>
-      <c r="AL59" s="33"/>
+      <c r="AK59" s="7"/>
+      <c r="AL59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="33" t="n">
+      <c r="A60" s="7" t="n">
         <v>54</v>
       </c>
-      <c r="B60" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C60" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D60" s="33" t="s">
-        <v>243</v>
-      </c>
-      <c r="E60" s="34" t="s">
+      <c r="B60" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E60" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="F60" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="G60" s="25" t="s">
+        <v>270</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="I60" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="F60" s="34" t="s">
-        <v>266</v>
-      </c>
-      <c r="G60" s="34" t="s">
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="O60" s="7"/>
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7"/>
+      <c r="R60" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="S60" s="7"/>
+      <c r="T60" s="7"/>
+      <c r="U60" s="7"/>
+      <c r="V60" s="7"/>
+      <c r="W60" s="7"/>
+      <c r="X60" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="H60" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="I60" s="33" t="s">
-        <v>262</v>
-      </c>
-      <c r="J60" s="35"/>
-      <c r="K60" s="35"/>
-      <c r="L60" s="35"/>
-      <c r="M60" s="33"/>
-      <c r="N60" s="33" t="s">
-        <v>268</v>
-      </c>
-      <c r="O60" s="33"/>
-      <c r="P60" s="33"/>
-      <c r="Q60" s="33"/>
-      <c r="R60" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="S60" s="33"/>
-      <c r="T60" s="33"/>
-      <c r="U60" s="33"/>
-      <c r="V60" s="33"/>
-      <c r="W60" s="33"/>
-      <c r="X60" s="17" t="s">
-        <v>264</v>
-      </c>
-      <c r="Y60" s="33"/>
-      <c r="Z60" s="33"/>
-      <c r="AA60" s="33"/>
-      <c r="AB60" s="33"/>
-      <c r="AC60" s="33"/>
-      <c r="AD60" s="36"/>
-      <c r="AE60" s="33"/>
-      <c r="AF60" s="33"/>
-      <c r="AG60" s="33"/>
-      <c r="AH60" s="33"/>
-      <c r="AI60" s="33"/>
-      <c r="AJ60" s="33" t="n">
+      <c r="Y60" s="7"/>
+      <c r="Z60" s="7"/>
+      <c r="AA60" s="7"/>
+      <c r="AB60" s="7"/>
+      <c r="AC60" s="7"/>
+      <c r="AD60" s="10"/>
+      <c r="AE60" s="7"/>
+      <c r="AF60" s="7"/>
+      <c r="AG60" s="7"/>
+      <c r="AH60" s="7"/>
+      <c r="AI60" s="7"/>
+      <c r="AJ60" s="7" t="n">
         <v>54</v>
       </c>
-      <c r="AK60" s="33"/>
-      <c r="AL60" s="33"/>
+      <c r="AK60" s="7"/>
+      <c r="AL60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="7" t="n">
@@ -6077,31 +5949,31 @@
         <v>39</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="E61" s="38"/>
-      <c r="F61" s="38" t="s">
-        <v>269</v>
-      </c>
-      <c r="G61" s="38" t="s">
-        <v>270</v>
+        <v>246</v>
+      </c>
+      <c r="E61" s="25"/>
+      <c r="F61" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="G61" s="25" t="s">
+        <v>273</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
       <c r="L61" s="9"/>
       <c r="M61" s="7"/>
-      <c r="N61" s="39"/>
+      <c r="N61" s="27"/>
       <c r="O61" s="7"/>
       <c r="P61" s="7"/>
       <c r="Q61" s="7"/>
       <c r="R61" s="7" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="S61" s="7"/>
       <c r="T61" s="7"/>

</xml_diff>

<commit_message>
DAS-677 - CCRU - Creation of Scenes for SOVI SOCVI
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - FT NS - CAP.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - FT NS - CAP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My folder\RED\POS\POS_2019-10-17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My folder\RED\POS\POS_2019-10-21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98155021-E399-4AB8-946E-D7CA6AB68B60}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FF3014-9E23-4102-9329-2485476777FC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="501" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Traditional Trade'!$A$1:$AL$56</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">'Traditional Trade'!$A$1:$AL$56</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="256">
   <si>
     <t>Sorting</t>
   </si>
@@ -219,9 +219,6 @@
     <t>Activation, Other</t>
   </si>
   <si>
-    <t>Panoramic Photo</t>
-  </si>
-  <si>
     <t>BINARY</t>
   </si>
   <si>
@@ -834,6 +831,12 @@
   </si>
   <si>
     <t>number of atomic KPI Passed on the same scene</t>
+  </si>
+  <si>
+    <t>Panoramic Photo, SS_Panoramic Photo</t>
+  </si>
+  <si>
+    <t>Panoramic photo of Cooler, SS_Panoramic photo of Cooler - Traditional Trade</t>
   </si>
 </sst>
 </file>
@@ -1294,10 +1297,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK56"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
+      <selection pane="bottomLeft" activeCell="Y56" sqref="Y56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1620,11 +1623,11 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB4" s="4"/>
       <c r="AC4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD4" s="6">
         <v>2.8000000000000001E-2</v>
@@ -1659,10 +1662,10 @@
         <v>44</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>51</v>
@@ -1674,10 +1677,10 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="3" t="s">
@@ -1692,11 +1695,11 @@
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB5" s="4"/>
       <c r="AC5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD5" s="6">
         <v>2.8000000000000001E-2</v>
@@ -1731,10 +1734,10 @@
         <v>44</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>51</v>
@@ -1746,10 +1749,10 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="3" t="s">
@@ -1764,11 +1767,11 @@
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB6" s="4"/>
       <c r="AC6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD6" s="6">
         <v>2.8000000000000001E-2</v>
@@ -1803,10 +1806,10 @@
         <v>44</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>51</v>
@@ -1818,10 +1821,10 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="3" t="s">
@@ -1836,11 +1839,11 @@
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB7" s="4"/>
       <c r="AC7" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD7" s="6">
         <v>2.8000000000000001E-2</v>
@@ -1875,10 +1878,10 @@
         <v>44</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>51</v>
@@ -1890,10 +1893,10 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="3" t="s">
@@ -1908,11 +1911,11 @@
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB8" s="4"/>
       <c r="AC8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD8" s="6">
         <v>2.8000000000000001E-2</v>
@@ -1947,10 +1950,10 @@
         <v>44</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>51</v>
@@ -1962,10 +1965,10 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="3" t="s">
@@ -1980,11 +1983,11 @@
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
       <c r="Y9" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB9" s="4"/>
       <c r="AC9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD9" s="6">
         <v>2.8000000000000001E-2</v>
@@ -2019,10 +2022,10 @@
         <v>44</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>51</v>
@@ -2034,7 +2037,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N10" s="3">
         <v>5449000064110</v>
@@ -2052,11 +2055,11 @@
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB10" s="4"/>
       <c r="AC10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD10" s="6">
         <v>2.8000000000000001E-2</v>
@@ -2091,10 +2094,10 @@
         <v>44</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>51</v>
@@ -2106,10 +2109,10 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="3" t="s">
@@ -2124,11 +2127,11 @@
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB11" s="4"/>
       <c r="AC11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD11" s="6">
         <v>2.8000000000000001E-2</v>
@@ -2163,10 +2166,10 @@
         <v>44</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>51</v>
@@ -2178,10 +2181,10 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="3" t="s">
@@ -2196,11 +2199,11 @@
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
       <c r="Y12" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB12" s="4"/>
       <c r="AC12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD12" s="6">
         <v>1.2999999999999999E-2</v>
@@ -2235,10 +2238,10 @@
         <v>44</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>51</v>
@@ -2250,7 +2253,7 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N13" s="3">
         <v>42099697</v>
@@ -2268,11 +2271,11 @@
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
       <c r="Y13" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB13" s="4"/>
       <c r="AC13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD13" s="6">
         <v>1.2999999999999999E-2</v>
@@ -2304,13 +2307,13 @@
         <v>40</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>47</v>
@@ -2362,13 +2365,13 @@
         <v>40</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>51</v>
@@ -2380,10 +2383,10 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="3" t="s">
@@ -2398,11 +2401,11 @@
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB15" s="4"/>
       <c r="AC15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD15" s="6">
         <v>1.7899999999999999E-2</v>
@@ -2434,13 +2437,13 @@
         <v>40</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>47</v>
@@ -2472,7 +2475,7 @@
         <v>17</v>
       </c>
       <c r="AK16" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AL16" s="3">
         <v>300</v>
@@ -2492,13 +2495,13 @@
         <v>40</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F17" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>51</v>
@@ -2510,10 +2513,10 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P17" s="4"/>
       <c r="Q17" s="3" t="s">
@@ -2528,11 +2531,11 @@
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB17" s="4"/>
       <c r="AC17" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD17" s="6">
         <v>1.7899999999999999E-2</v>
@@ -2564,13 +2567,13 @@
         <v>40</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>51</v>
@@ -2582,7 +2585,7 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N18" s="3">
         <v>5060335632906</v>
@@ -2600,11 +2603,11 @@
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
       <c r="Y18" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB18" s="4"/>
       <c r="AC18" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD18" s="6">
         <v>1.7899999999999999E-2</v>
@@ -2636,13 +2639,13 @@
         <v>40</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>47</v>
@@ -2674,7 +2677,7 @@
         <v>20</v>
       </c>
       <c r="AK19" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AL19" s="3">
         <v>300</v>
@@ -2694,13 +2697,13 @@
         <v>40</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F20" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>51</v>
@@ -2712,10 +2715,10 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="N20" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="3" t="s">
@@ -2730,11 +2733,11 @@
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB20" s="4"/>
       <c r="AC20" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD20" s="6">
         <v>1.7899999999999999E-2</v>
@@ -2766,13 +2769,13 @@
         <v>40</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>51</v>
@@ -2784,10 +2787,10 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P21" s="4"/>
       <c r="Q21" s="3" t="s">
@@ -2802,11 +2805,11 @@
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
       <c r="Y21" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB21" s="4"/>
       <c r="AC21" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD21" s="6">
         <v>1.2999999999999999E-2</v>
@@ -2838,13 +2841,13 @@
         <v>40</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F22" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>47</v>
@@ -2876,7 +2879,7 @@
         <v>23</v>
       </c>
       <c r="AK22" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AL22" s="3">
         <v>300</v>
@@ -2896,13 +2899,13 @@
         <v>40</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>51</v>
@@ -2914,10 +2917,10 @@
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P23" s="4"/>
       <c r="Q23" s="3" t="s">
@@ -2932,11 +2935,11 @@
       <c r="W23" s="4"/>
       <c r="X23" s="4"/>
       <c r="Y23" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB23" s="4"/>
       <c r="AC23" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD23" s="6">
         <v>1.788E-2</v>
@@ -2968,13 +2971,13 @@
         <v>40</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>51</v>
@@ -2986,10 +2989,10 @@
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P24" s="4"/>
       <c r="Q24" s="3" t="s">
@@ -3004,11 +3007,11 @@
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
       <c r="Y24" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB24" s="4"/>
       <c r="AC24" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD24" s="6">
         <v>1.788E-2</v>
@@ -3040,13 +3043,13 @@
         <v>40</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F25" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>51</v>
@@ -3058,10 +3061,10 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P25" s="4"/>
       <c r="Q25" s="3" t="s">
@@ -3076,11 +3079,11 @@
       <c r="W25" s="4"/>
       <c r="X25" s="4"/>
       <c r="Y25" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB25" s="4"/>
       <c r="AC25" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD25" s="6">
         <v>1.788E-2</v>
@@ -3112,13 +3115,13 @@
         <v>40</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F26" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>51</v>
@@ -3130,10 +3133,10 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P26" s="4"/>
       <c r="Q26" s="3" t="s">
@@ -3148,11 +3151,11 @@
       <c r="W26" s="4"/>
       <c r="X26" s="4"/>
       <c r="Y26" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB26" s="4"/>
       <c r="AC26" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD26" s="6">
         <v>1.788E-2</v>
@@ -3184,13 +3187,13 @@
         <v>40</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F27" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>51</v>
@@ -3202,10 +3205,10 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P27" s="4"/>
       <c r="Q27" s="3" t="s">
@@ -3220,11 +3223,11 @@
       <c r="W27" s="4"/>
       <c r="X27" s="4"/>
       <c r="Y27" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB27" s="4"/>
       <c r="AC27" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD27" s="6">
         <v>1.788E-2</v>
@@ -3256,13 +3259,13 @@
         <v>40</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>51</v>
@@ -3274,10 +3277,10 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P28" s="4"/>
       <c r="Q28" s="3" t="s">
@@ -3292,11 +3295,11 @@
       <c r="W28" s="4"/>
       <c r="X28" s="4"/>
       <c r="Y28" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB28" s="4"/>
       <c r="AC28" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD28" s="6">
         <v>1.2999999999999999E-2</v>
@@ -3328,13 +3331,13 @@
         <v>40</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F29" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>51</v>
@@ -3346,10 +3349,10 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P29" s="4"/>
       <c r="Q29" s="3" t="s">
@@ -3364,11 +3367,11 @@
       <c r="W29" s="4"/>
       <c r="X29" s="4"/>
       <c r="Y29" s="3" t="s">
-        <v>57</v>
+        <v>254</v>
       </c>
       <c r="AB29" s="4"/>
       <c r="AC29" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD29" s="6">
         <v>1.2999999999999999E-2</v>
@@ -3401,10 +3404,10 @@
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>40</v>
@@ -3452,10 +3455,10 @@
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>40</v>
@@ -3504,16 +3507,16 @@
         <v>40</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="G32" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="G32" s="7" t="s">
-        <v>137</v>
-      </c>
       <c r="H32" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="3">
@@ -3529,13 +3532,13 @@
       </c>
       <c r="R32" s="4"/>
       <c r="W32" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X32" s="4"/>
       <c r="Y32" s="4"/>
       <c r="AB32" s="4"/>
       <c r="AC32" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD32" s="6">
         <v>0.15</v>
@@ -3549,7 +3552,7 @@
         <v>32</v>
       </c>
       <c r="AK32" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AL32" s="3">
         <v>303</v>
@@ -3569,13 +3572,13 @@
         <v>40</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F33" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>51</v>
@@ -3587,26 +3590,26 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="N33" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="P33" s="4"/>
       <c r="Q33" s="3" t="s">
         <v>54</v>
       </c>
       <c r="R33" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="W33" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X33" s="4"/>
       <c r="Y33" s="4"/>
       <c r="AB33" s="4"/>
       <c r="AC33" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD33" s="4"/>
       <c r="AG33" s="4"/>
@@ -3636,16 +3639,16 @@
         <v>40</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F34" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="H34" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="3">
@@ -3661,13 +3664,13 @@
       </c>
       <c r="R34" s="4"/>
       <c r="W34" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X34" s="4"/>
       <c r="Y34" s="4"/>
       <c r="AB34" s="4"/>
       <c r="AC34" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD34" s="4"/>
       <c r="AG34" s="4"/>
@@ -3679,7 +3682,7 @@
         <v>34</v>
       </c>
       <c r="AK34" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AL34" s="3">
         <v>32</v>
@@ -3699,23 +3702,23 @@
         <v>40</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F35" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="H35" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N35" s="3">
         <v>4607042434877</v>
@@ -3728,18 +3731,18 @@
         <v>55</v>
       </c>
       <c r="W35" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X35" s="4"/>
       <c r="Y35" s="4"/>
       <c r="AB35" s="4"/>
       <c r="AC35" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD35" s="4"/>
       <c r="AG35" s="4"/>
       <c r="AH35" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AI35" s="3">
         <v>4</v>
@@ -3766,23 +3769,23 @@
         <v>40</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F36" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="H36" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N36" s="3">
         <v>4607042434891</v>
@@ -3795,18 +3798,18 @@
         <v>55</v>
       </c>
       <c r="W36" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X36" s="4"/>
       <c r="Y36" s="4"/>
       <c r="AB36" s="4"/>
       <c r="AC36" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD36" s="4"/>
       <c r="AG36" s="4"/>
       <c r="AH36" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AI36" s="3">
         <v>4</v>
@@ -3834,10 +3837,10 @@
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>40</v>
@@ -3866,7 +3869,7 @@
         <v>310</v>
       </c>
       <c r="AK37" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AL37" s="4"/>
     </row>
@@ -3885,10 +3888,10 @@
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>40</v>
@@ -3937,16 +3940,16 @@
         <v>40</v>
       </c>
       <c r="E39" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="H39" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -3956,7 +3959,7 @@
       <c r="N39" s="4"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R39" s="4"/>
       <c r="W39" s="4"/>
@@ -3964,14 +3967,14 @@
       <c r="Y39" s="4"/>
       <c r="AB39" s="4"/>
       <c r="AC39" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AD39" s="6">
         <v>0.24</v>
       </c>
       <c r="AG39" s="4"/>
       <c r="AH39" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AI39" s="3">
         <v>2</v>
@@ -3980,7 +3983,7 @@
         <v>36</v>
       </c>
       <c r="AK39" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AL39" s="3">
         <v>311</v>
@@ -4000,16 +4003,16 @@
         <v>40</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F40" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="H40" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="3">
@@ -4020,30 +4023,30 @@
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="N40" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="N40" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
       <c r="R40" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="W40" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="W40" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="X40" s="4"/>
       <c r="AB40" s="4"/>
       <c r="AC40" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD40" s="4"/>
       <c r="AG40" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AH40" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="AH40" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="AI40" s="3">
         <v>3</v>
@@ -4070,16 +4073,16 @@
         <v>40</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F41" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="3">
@@ -4088,24 +4091,24 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N41" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
       <c r="R41" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="W41" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="X41" s="4"/>
       <c r="Y41" s="4"/>
       <c r="AB41" s="4"/>
       <c r="AC41" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD41" s="4"/>
       <c r="AG41" s="4"/>
@@ -4136,10 +4139,10 @@
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>40</v>
@@ -4168,7 +4171,7 @@
         <v>312</v>
       </c>
       <c r="AK42" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AL42" s="3">
         <v>310</v>
@@ -4188,16 +4191,16 @@
         <v>40</v>
       </c>
       <c r="E43" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="3">
@@ -4207,32 +4210,32 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
       <c r="N43" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="W43" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="W43" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="X43" s="3" t="s">
-        <v>188</v>
+        <v>255</v>
       </c>
       <c r="Y43" s="4"/>
       <c r="AB43" s="4"/>
       <c r="AC43" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD43" s="6">
         <v>0.04</v>
       </c>
       <c r="AG43" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AH43" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AI43" s="3">
         <v>2</v>
@@ -4259,16 +4262,16 @@
         <v>40</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F44" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="H44" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
@@ -4279,32 +4282,32 @@
         <v>15</v>
       </c>
       <c r="M44" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="N44" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="N44" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
       <c r="R44" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="W44" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="W44" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="X44" s="4"/>
       <c r="AB44" s="4"/>
       <c r="AC44" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD44" s="6">
         <v>0.04</v>
       </c>
       <c r="AG44" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AH44" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AI44" s="3">
         <v>2</v>
@@ -4331,13 +4334,13 @@
         <v>40</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F45" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>47</v>
@@ -4348,25 +4351,25 @@
       <c r="N45" s="4"/>
       <c r="P45" s="4"/>
       <c r="Q45" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R45" s="4"/>
       <c r="W45" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="X45" s="4"/>
       <c r="AB45" s="4"/>
       <c r="AC45" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AD45" s="6">
         <v>0.04</v>
       </c>
       <c r="AG45" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AH45" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AI45" s="3">
         <v>2</v>
@@ -4375,7 +4378,7 @@
         <v>42</v>
       </c>
       <c r="AK45" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AL45" s="3">
         <v>312</v>
@@ -4396,49 +4399,49 @@
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="H46" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="3">
         <v>0.4</v>
       </c>
       <c r="M46" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="N46" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="N46" s="3" t="s">
-        <v>203</v>
-      </c>
       <c r="P46" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q46" s="3" t="s">
         <v>54</v>
       </c>
       <c r="R46" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="W46" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="X46" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AB46" s="4"/>
       <c r="AC46" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD46" s="4"/>
       <c r="AG46" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AH46" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AI46" s="3">
         <v>3</v>
@@ -4466,13 +4469,13 @@
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>206</v>
-      </c>
       <c r="H47" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I47" s="4"/>
       <c r="J47" s="3">
@@ -4482,23 +4485,23 @@
       <c r="N47" s="4"/>
       <c r="P47" s="4"/>
       <c r="Q47" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R47" s="4"/>
       <c r="W47" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="X47" s="4"/>
       <c r="AB47" s="4"/>
       <c r="AC47" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD47" s="4"/>
       <c r="AG47" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AH47" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AI47" s="3">
         <v>3</v>
@@ -4507,7 +4510,7 @@
         <v>45</v>
       </c>
       <c r="AK47" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AL47" s="3">
         <v>42</v>
@@ -4528,10 +4531,10 @@
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>51</v>
@@ -4541,38 +4544,38 @@
         <v>4</v>
       </c>
       <c r="M48" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="N48" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="N48" s="3" t="s">
-        <v>211</v>
-      </c>
       <c r="P48" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q48" s="3" t="s">
         <v>54</v>
       </c>
       <c r="R48" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="W48" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="X48" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AB48" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AC48" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD48" s="4"/>
       <c r="AG48" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AH48" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AI48" s="3">
         <v>4</v>
@@ -4600,10 +4603,10 @@
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>214</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>51</v>
@@ -4613,38 +4616,38 @@
         <v>4</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N49" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q49" s="3" t="s">
         <v>54</v>
       </c>
       <c r="R49" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="W49" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="X49" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AB49" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AC49" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD49" s="4"/>
       <c r="AG49" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AH49" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AI49" s="3">
         <v>4</v>
@@ -4672,45 +4675,45 @@
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="H50" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="I50" s="4"/>
       <c r="J50" s="3">
         <v>2</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N50" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q50" s="3" t="s">
         <v>54</v>
       </c>
       <c r="R50" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="W50" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="W50" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="X50" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AC50" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD50" s="4"/>
       <c r="AG50" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AH50" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AI50" s="3">
         <v>3</v>
@@ -4737,39 +4740,39 @@
         <v>40</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F51" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="H51" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="I51" s="4"/>
       <c r="N51" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="R51" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="R51" s="3" t="s">
+      <c r="W51" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="W51" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="X51" s="4"/>
       <c r="AC51" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AD51" s="6">
         <v>0.04</v>
       </c>
       <c r="AG51" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AH51" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AI51" s="3">
         <v>2</v>
@@ -4793,26 +4796,26 @@
         <v>39</v>
       </c>
       <c r="D52" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="G52" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="H52" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="I52" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="N52" s="4"/>
       <c r="R52" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="W52" s="4"/>
       <c r="X52" s="4"/>
@@ -4820,7 +4823,7 @@
         <v>50</v>
       </c>
       <c r="AK52" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="53" spans="1:38" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4834,34 +4837,34 @@
         <v>39</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E53" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="G53" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="H53" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="I53" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="N53" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="I53" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="N53" s="3" t="s">
+      <c r="R53" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="R53" s="3" t="s">
-        <v>235</v>
-      </c>
       <c r="W53" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="X53" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AJ53" s="3">
         <v>51</v>
@@ -4878,31 +4881,31 @@
         <v>39</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E54" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="G54" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="G54" s="3" t="s">
+      <c r="H54" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="I54" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="I54" s="3" t="s">
+      <c r="N54" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="N54" s="3" t="s">
+      <c r="R54" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="X54" s="5" t="s">
         <v>241</v>
-      </c>
-      <c r="R54" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="X54" s="5" t="s">
-        <v>242</v>
       </c>
       <c r="AJ54" s="3">
         <v>52</v>
@@ -4919,31 +4922,31 @@
         <v>39</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E55" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="F55" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="G55" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="H55" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="N55" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H55" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="N55" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="R55" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="X55" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AJ55" s="3">
         <v>54</v>
@@ -4960,22 +4963,22 @@
         <v>39</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F56" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G56" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="H56" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="I56" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="H56" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>249</v>
-      </c>
       <c r="R56" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AJ56" s="3">
         <v>313</v>

</xml_diff>